<commit_message>
link entre back-end e planilha excel concluído
</commit_message>
<xml_diff>
--- a/BaseDados.xlsx
+++ b/BaseDados.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CEB1594F-9513-4228-A534-29FFA356828B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ti2\Downloads\site-novos-negocios\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3519AFC8-F58E-426B-9400-854980DD6F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>ORIGEM</t>
   </si>
@@ -43,14 +48,37 @@
   </si>
   <si>
     <t>INTERNO</t>
+  </si>
+  <si>
+    <t>Origem lead - 11</t>
+  </si>
+  <si>
+    <t>PRISCYLLA</t>
+  </si>
+  <si>
+    <t>PROSP MAURO</t>
+  </si>
+  <si>
+    <t>VISÃO CEDENTE</t>
+  </si>
+  <si>
+    <t>ALEX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -78,8 +106,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,40 +449,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="12.140625" customWidth="1"/>
     <col min="5" max="5" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>30</v>
       </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>29</v>
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>